<commit_message>
Actualización nombre imágenes, excel y sql bd
</commit_message>
<xml_diff>
--- a/Desarrollo_Web_en_Entorno_Servidor/Segundo_Trimestre/Tarea Final/doc/Lista_Juegos.xlsx
+++ b/Desarrollo_Web_en_Entorno_Servidor/Segundo_Trimestre/Tarea Final/doc/Lista_Juegos.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\Documents\GitHub 2-DAW\2-DAW\Desarrollo_Web_en_Entorno_Servidor\Segundo_Trimestre\Tarea Final\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\OneDrive\Documentos\2-DAW\Desarrollo_Web_en_Entorno_Servidor\Segundo_Trimestre\Tarea Final\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A06E0B-5B94-43E0-8E44-57F0212BBA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C85275-52A7-4629-B274-F43574E9DB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12BFB003-D532-4BC6-8A1B-2759774178E0}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{12BFB003-D532-4BC6-8A1B-2759774178E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -583,6 +583,8 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,8 +594,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -931,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A4B632-89C8-4569-BC42-C36A200D3EFE}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,1040 +941,1181 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="3" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="3" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="3" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="3" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="3" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="3" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="3" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="3" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="3" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="3" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="3" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="3" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="3" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="3" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="3" t="s">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2" t="s">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="3" t="s">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="3" t="s">
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2" t="s">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="2" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="3" t="s">
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="2" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="2" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="2" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="2" t="s">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="2" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="2" t="s">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="2" t="s">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="2" t="s">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="3" t="s">
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="2" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="2" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="3" t="s">
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="2" t="s">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="2" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="3" t="s">
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="2" t="s">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="2" t="s">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1" t="s">
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="2" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1" t="s">
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="2" t="s">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1" t="s">
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="2" t="s">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1" t="s">
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="2" t="s">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="3" t="s">
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="2" t="s">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="3" t="s">
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="153">
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="H51:L51"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="H49:L49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="H47:L47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="H48:L48"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="H45:L45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="H46:L46"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="H24:L24"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:L6"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="H3:L3"/>
@@ -1987,147 +2128,6 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="H23:L23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="H24:L24"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="H22:L22"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="H25:L25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="H33:L33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:G40"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="H47:L47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="H48:L48"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="H45:L45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="H46:L46"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="H51:L51"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="H49:L49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="H50:L50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{82C146CC-D025-4C6B-8FAB-E854A7F78050}"/>

</xml_diff>